<commit_message>
we should add shading surfaces when possible
</commit_message>
<xml_diff>
--- a/A_prepost_processing/AllCases/Vancouver_Rural_WithShading_WithCoolingcomparison.xlsx
+++ b/A_prepost_processing/AllCases/Vancouver_Rural_WithShading_WithCoolingcomparison.xlsx
@@ -20971,7 +20971,7 @@
         <v>101602.196</v>
       </c>
       <c r="Q331">
-        <v>20.87547880085168</v>
+        <v>20.87547880085162</v>
       </c>
       <c r="R331">
         <v>294.249</v>
@@ -30519,7 +30519,7 @@
         <v>101606.466</v>
       </c>
       <c r="Q485">
-        <v>15.37919827184396</v>
+        <v>15.37919827184402</v>
       </c>
       <c r="R485">
         <v>288.822</v>
@@ -81306,7 +81306,7 @@
         <v>101608.998</v>
       </c>
       <c r="T1304">
-        <v>12.69697232936869</v>
+        <v>12.69697232936875</v>
       </c>
     </row>
     <row r="1305" spans="1:20">
@@ -92761,9 +92761,6 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
-        <v>32.61</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>